<commit_message>
update seluruh screenshot & tabel
</commit_message>
<xml_diff>
--- a/tugas7/screenshot/table_bench.xlsx
+++ b/tugas7/screenshot/table_bench.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/103eeb4ae6ff65b9/Documents/Kuliah/Semester VI/Pemrograman Jaringan/progjar-b-its-2020/tugas7/screenshot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BF38038-AA32-444E-9437-7D4B37E80AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{3BF38038-AA32-444E-9437-7D4B37E80AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B85B69D3-D184-40BE-B100-7FB3F7F0E45E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4095" windowWidth="16965" windowHeight="11625" xr2:uid="{D60C7181-DC52-4154-AF1C-312B725FE562}"/>
+    <workbookView xWindow="2070" yWindow="3840" windowWidth="16965" windowHeight="11625" xr2:uid="{D60C7181-DC52-4154-AF1C-312B725FE562}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>No Test</t>
   </si>
@@ -62,58 +62,145 @@
     <t>Transfer rate</t>
   </si>
   <si>
-    <t>1, 5, 10</t>
-  </si>
-  <si>
-    <t>0.112s</t>
-  </si>
-  <si>
     <t>1360 bytes</t>
   </si>
   <si>
-    <t>11.161 ms</t>
-  </si>
-  <si>
-    <t>11.90 Kbytes/s</t>
-  </si>
-  <si>
-    <t>1, 10, 30, 50</t>
-  </si>
-  <si>
-    <t>1.012s</t>
-  </si>
-  <si>
     <t>6800 bytes</t>
   </si>
   <si>
-    <t>49.42 #/s</t>
-  </si>
-  <si>
-    <t>20.236 ms</t>
-  </si>
-  <si>
-    <t>6.56 Kbytes/s</t>
-  </si>
-  <si>
-    <t>89.60 #/s</t>
-  </si>
-  <si>
-    <t>1, 10, 50, 100</t>
-  </si>
-  <si>
-    <t>2.806 s</t>
-  </si>
-  <si>
     <t>13600 bytes</t>
   </si>
   <si>
-    <t>35.64 #/s</t>
-  </si>
-  <si>
-    <t>28.058 ms</t>
-  </si>
-  <si>
-    <t>4.73 Kbytes/s</t>
+    <t>0.119s</t>
+  </si>
+  <si>
+    <t>84.11 #/s</t>
+  </si>
+  <si>
+    <t>11.890 ms</t>
+  </si>
+  <si>
+    <t>11.17 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.049s</t>
+  </si>
+  <si>
+    <t>203.10 #/s</t>
+  </si>
+  <si>
+    <t>4.924 ms</t>
+  </si>
+  <si>
+    <t>26.97 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.039s</t>
+  </si>
+  <si>
+    <t>259.67 #/s</t>
+  </si>
+  <si>
+    <t>3.851 ms</t>
+  </si>
+  <si>
+    <t>34.49 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.527s</t>
+  </si>
+  <si>
+    <t>94.82 #/s</t>
+  </si>
+  <si>
+    <t>10.547 ms</t>
+  </si>
+  <si>
+    <t>12.59 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.297 s</t>
+  </si>
+  <si>
+    <t>168.38 #/s</t>
+  </si>
+  <si>
+    <t>5.939 ms</t>
+  </si>
+  <si>
+    <t>22.36 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.360 s</t>
+  </si>
+  <si>
+    <t>139.00 #/s</t>
+  </si>
+  <si>
+    <t>7.194 ms</t>
+  </si>
+  <si>
+    <t>18.46 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.451 s</t>
+  </si>
+  <si>
+    <t>110.78 #/s</t>
+  </si>
+  <si>
+    <t>9.027 ms</t>
+  </si>
+  <si>
+    <t>14.71 Kbytes/s</t>
+  </si>
+  <si>
+    <t>1.408 s</t>
+  </si>
+  <si>
+    <t>71.04 #/s</t>
+  </si>
+  <si>
+    <t>14.076 ms</t>
+  </si>
+  <si>
+    <t>9.44 Kbtes/s</t>
+  </si>
+  <si>
+    <t>1.113 s</t>
+  </si>
+  <si>
+    <t>89.85 #/s</t>
+  </si>
+  <si>
+    <t>11.129 ms</t>
+  </si>
+  <si>
+    <t>11.93 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.925 s</t>
+  </si>
+  <si>
+    <t>108.15 #/s</t>
+  </si>
+  <si>
+    <t>9.247 ms</t>
+  </si>
+  <si>
+    <t>14.36 Kbytes/s</t>
+  </si>
+  <si>
+    <t>0.930 s</t>
+  </si>
+  <si>
+    <t>107.58 #/s</t>
+  </si>
+  <si>
+    <t>9.295 ms</t>
+  </si>
+  <si>
+    <t>14.29 Kbytes/s</t>
   </si>
 </sst>
 </file>
@@ -164,23 +251,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,146 +586,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545CFC2B-D6BD-4203-812C-008A6BDC1F61}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5">
         <v>10</v>
       </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3">
+        <v>50</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="G9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="5">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3">
+        <v>100</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="5">
         <v>50</v>
       </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3">
         <v>100</v>
       </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>26</v>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="5">
+        <v>100</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="3">
+        <v>100</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>